<commit_message>
Perubahan tampilan pada filter, dashboard
</commit_message>
<xml_diff>
--- a/public/template_mahasiswa.xlsx
+++ b/public/template_mahasiswa.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>nomor_induk</t>
   </si>
@@ -32,19 +32,13 @@
     <t>nama</t>
   </si>
   <si>
-    <t>semester</t>
-  </si>
-  <si>
     <t>jam_alpha</t>
   </si>
   <si>
-    <t>jam_kompen</t>
+    <t>prodi</t>
   </si>
   <si>
-    <t>jam_kompen_selesai</t>
-  </si>
-  <si>
-    <t>prodi</t>
+    <t>periode_tahun</t>
   </si>
 </sst>
 </file>
@@ -371,19 +365,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="A1:XFD1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -391,20 +388,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="F1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>